<commit_message>
Add the flood warning map, issue #168
</commit_message>
<xml_diff>
--- a/workflow/CurrentConditions/Environment-Floods/data/flood-orgs.xlsx
+++ b/workflow/CurrentConditions/Environment-Floods/data/flood-orgs.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
-  <si>
-    <t>This Excel workbook is an initial enventory of educational organizations that will be shown on the Basin Entities / Education - Organization map.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Organization</t>
   </si>
@@ -112,6 +109,24 @@
   </si>
   <si>
     <t>FloodplainRegWebpage</t>
+  </si>
+  <si>
+    <t>Boxelder Regional Stormwater Authority</t>
+  </si>
+  <si>
+    <t>IGA</t>
+  </si>
+  <si>
+    <t>Stormwater - Authority</t>
+  </si>
+  <si>
+    <t>https://www.boxelderauthority.org/</t>
+  </si>
+  <si>
+    <t>This Excel workbook is an initial inventory of stormwater/floodplain organizations that will be shown on the Current Conditions / Environment - Floods map.</t>
+  </si>
+  <si>
+    <t>Coordinates are for consulting company.</t>
   </si>
 </sst>
 </file>
@@ -445,15 +460,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -466,10 +479,10 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="19" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="19" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,57 +502,57 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>-104.69286</v>
@@ -550,22 +563,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>-105.08011999999999</v>
@@ -576,22 +589,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <v>-105.11454999999999</v>
@@ -602,22 +615,22 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <v>-105.07980000000001</v>
@@ -627,7 +640,33 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E6" s="1"/>
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>-105.08399</v>
+      </c>
+      <c r="H6">
+        <v>40.40446</v>
+      </c>
+      <c r="K6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E7" s="1"/>
@@ -674,8 +713,9 @@
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>